<commit_message>
GettingStarted skeleton. Needs writing
</commit_message>
<xml_diff>
--- a/Docs/LMT70-BOM.xlsx
+++ b/Docs/LMT70-BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17200" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>40 Pos Male Header Pins</t>
-  </si>
-  <si>
     <t>LMT70</t>
   </si>
   <si>
@@ -131,14 +128,18 @@
   </si>
   <si>
     <t>296-42088-1-ND</t>
+  </si>
+  <si>
+    <t>1/8 of 40 Pos Male Header Pins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -220,7 +221,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="386">
+  <cellStyleXfs count="388">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -607,8 +608,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -621,6 +624,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -676,7 +680,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="386">
+  <cellStyles count="388">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -874,6 +878,7 @@
     <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1062,6 +1067,7 @@
     <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1393,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1414,190 +1420,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="16" t="s">
+      <c r="A1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="17">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="18">
         <f>SUM(M3:M5)</f>
-        <v>4.0299999999999994</v>
+        <v>3.3824999999999998</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="21" customFormat="1" ht="33">
-      <c r="A3" s="10">
+    <row r="3" spans="1:13" s="22" customFormat="1" ht="33">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="11">
+      <c r="K3" s="12">
         <v>1</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="15">
         <v>3.19</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="20">
         <f>K3*L3</f>
         <v>3.19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="21" customFormat="1">
-      <c r="A4" s="10">
+    <row r="4" spans="1:13" s="22" customFormat="1">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1</v>
+      </c>
+      <c r="L4" s="15">
+        <f>0.74/8</f>
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="M4" s="20">
+        <f t="shared" ref="M4:M5" si="0">K4*L4</f>
+        <v>9.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="22" customFormat="1">
+      <c r="A5" s="22">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="E5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="12">
+      <c r="J5" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="22">
         <v>1</v>
       </c>
-      <c r="L4" s="14">
-        <v>0.74</v>
-      </c>
-      <c r="M4" s="19">
-        <f t="shared" ref="M4:M5" si="0">K4*L4</f>
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="21" customFormat="1">
-      <c r="A5" s="21">
-        <v>3</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="21">
-        <v>1</v>
-      </c>
-      <c r="L5" s="20">
+      <c r="L5" s="21">
         <v>0.1</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="20">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -1607,6 +1614,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="I9" s="2"/>
+      <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13">
       <c r="I10" s="2"/>

</xml_diff>